<commit_message>
CalculateAmortizationDurationTest working with decision table method
</commit_message>
<xml_diff>
--- a/decision-table-drools-geode/src/test/resources/rules/calculateAmortizationDuration.drl.xlsx
+++ b/decision-table-drools-geode/src/test/resources/rules/calculateAmortizationDuration.drl.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB81BFF-2E94-8440-A403-3A4CC620CA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CECCB56-78A5-3847-94F8-580D451198FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>RuleSet</t>
   </si>
@@ -53,9 +53,6 @@
     <t>false</t>
   </si>
   <si>
-    <t>$vehicle:Vehicle</t>
-  </si>
-  <si>
     <t>rules</t>
   </si>
   <si>
@@ -80,12 +77,6 @@
     <t>null</t>
   </si>
   <si>
-    <t>$vehicle.getStartDate()</t>
-  </si>
-  <si>
-    <t>$vehicle.getOldVehiclesAmortizationPeriod() - (double)DateUtil.dateDifMonths($vehicle.getPurchaseDate(), $vehicle.getStartDate()) / 12</t>
-  </si>
-  <si>
     <t>Amortissment &lt; 0</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
     <t>Purchase Date + Old Vehicle Amortization Period</t>
   </si>
   <si>
-    <t>Vehicle</t>
-  </si>
-  <si>
     <t>getPurchaseDate() != $param</t>
   </si>
   <si>
@@ -113,10 +101,22 @@
     <t>com.kc.poc.drools.util.DateUtil, com.kc.poc.drools.fact.Vehicle, java.time.LocalDate</t>
   </si>
   <si>
-    <t>getNewVehiclesAmortizationPeriod()</t>
-  </si>
-  <si>
-    <t>setAmortizationDuration($param);</t>
+    <t>vehicle:Vehicle</t>
+  </si>
+  <si>
+    <t>vehicle.setAmortizationDuration($param);</t>
+  </si>
+  <si>
+    <t>vehicle.getOldVehiclesAmortizationPeriod() - (double)DateUtil.dateDifMonths(vehicle.getPurchaseDate(), vehicle.getStartDate()) / 12</t>
+  </si>
+  <si>
+    <t>vehicle.getStartDate()</t>
+  </si>
+  <si>
+    <t>vehicle.getNewVehiclesAmortizationPeriod()</t>
+  </si>
+  <si>
+    <t>true, false</t>
   </si>
 </sst>
 </file>
@@ -166,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -189,11 +189,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -201,6 +238,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -520,7 +566,7 @@
     <col min="5" max="5" width="33.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="37.1640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="81" style="1" customWidth="1"/>
-    <col min="8" max="8" width="108.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="115.33203125" style="1" customWidth="1"/>
     <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -529,7 +575,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -537,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -580,46 +626,36 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -630,19 +666,19 @@
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>9</v>
@@ -650,7 +686,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>10</v>
@@ -668,33 +704,35 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -714,6 +752,9 @@
       <c r="A24" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B7:G7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>